<commit_message>
[5_1_gamma] Added full excel
</commit_message>
<xml_diff>
--- a/5.1/src/gamma.xlsx
+++ b/5.1/src/gamma.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\!MIPT\Labs\PhysLabV\5.1\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B712203-B268-4A10-9FD2-2BB7C8CF8A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96325859-1CD8-4807-9024-1EB5D38E77E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="27">
   <si>
     <t>N_0</t>
   </si>
@@ -65,11 +66,57 @@
   <si>
     <t>ln</t>
   </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>\sigma_l</t>
+  </si>
+  <si>
+    <t>&lt;N&gt;</t>
+  </si>
+  <si>
+    <t>\sigma_{&lt;N&gt;}</t>
+  </si>
+  <si>
+    <t>&lt;N&gt;-N_ф</t>
+  </si>
+  <si>
+    <t>\sigma</t>
+  </si>
+  <si>
+    <t>\mu</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>\sigma_a</t>
+  </si>
+  <si>
+    <t>\sigma_{\mu}</t>
+  </si>
+  <si>
+    <t>\rho</t>
+  </si>
+  <si>
+    <t>\mu'</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>av</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -105,10 +152,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -226,11 +277,175 @@
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="ru-RU"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Лист1!$I$14:$I$18</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.05</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.15000000000000002</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.25</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Лист1!$I$14:$I$18</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.05</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.15000000000000002</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.25</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Лист1!$O$14:$O$18</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>8.3917093952487511E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.0609587274816201E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.5417534653339705E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.1046096630728626E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>6.7054707701933213E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Лист1!$O$14:$O$18</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>8.3917093952487511E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.0609587274816201E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.5417534653339705E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.1046096630728626E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>6.7054707701933213E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Лист1!$E$2:$I$2</c:f>
+              <c:f>Лист1!$I$2:$M$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -254,7 +469,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$E$10:$I$10</c:f>
+              <c:f>Лист1!$I$10:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -279,7 +494,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6D9B-4384-8DB1-2615B6C994BA}"/>
+              <c16:uniqueId val="{00000001-5F69-44A1-AF82-87E1B8AD0173}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -618,8 +833,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.1955922051378985E-2"/>
-          <c:y val="0.14592306188648596"/>
+          <c:x val="7.696410655519427E-2"/>
+          <c:y val="0.14592304130880515"/>
           <c:w val="0.87843417547300207"/>
           <c:h val="0.67938115682571032"/>
         </c:manualLayout>
@@ -671,7 +886,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Лист1!$M$2:$Q$2</c:f>
+              <c:f>Лист1!$V$16:$Z$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -695,7 +910,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$M$10:$Q$10</c:f>
+              <c:f>Лист1!$V$24:$Z$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -720,7 +935,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7060-4745-8124-2D76AF4C91C3}"/>
+              <c16:uniqueId val="{00000001-474A-4877-996B-C1E1624C82F6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1161,7 +1376,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-56CD-4995-9B96-39F730567B8A}"/>
+              <c16:uniqueId val="{00000001-A982-4FF5-8AA6-2A31EF58E937}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1553,7 +1768,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Лист1!$F$15:$H$15</c:f>
+              <c:f>Лист1!$B$15:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1571,7 +1786,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$F$22:$H$22</c:f>
+              <c:f>Лист1!$B$22:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1590,7 +1805,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C072-4849-94AE-30624D793036}"/>
+              <c16:uniqueId val="{00000001-CD31-4F29-8F7E-C2CD2DB33ADD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4081,27 +4296,29 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>533399</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>94297</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>125729</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>64770</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>207645</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>145733</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Диаграмма 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{067B8460-6C7A-43D1-8BE0-8779E3629B87}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C3B6D19-D4F2-46E0-97E6-CE0251A31DD2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4117,23 +4334,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>207645</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>145733</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1905</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>140018</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Диаграмма 3">
+        <xdr:cNvPr id="3" name="Диаграмма 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D680038-9685-4967-B99C-AFDAACE7D762}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F5CC533-804A-480D-ADD3-F0E767A3E87B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4155,23 +4372,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>207645</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>141923</xdr:rowOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>136208</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Диаграмма 4">
+        <xdr:cNvPr id="4" name="Диаграмма 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3090B97-3037-4301-9382-F8BA7C029CD1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0107038-FB28-4E97-BBA2-D67DD26181AF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4193,23 +4410,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>207645</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>141923</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>49530</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>113348</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Диаграмма 5">
+        <xdr:cNvPr id="5" name="Диаграмма 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17D80CC5-8173-4EB9-9059-AA747D15C8B6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F62895E-4FFB-41F9-8770-C0B439D90D95}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4683,49 +4900,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X23"/>
+  <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="G1">
+      <c r="K1">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="I1">
-        <v>0.05</v>
-      </c>
-      <c r="M1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1">
-        <v>1</v>
-      </c>
-      <c r="P1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1">
+      <c r="M1">
         <v>0.05</v>
       </c>
       <c r="T1" t="s">
@@ -4744,7 +4949,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>176871</v>
       </c>
@@ -4755,51 +4960,28 @@
         <f>SQRT(B2)</f>
         <v>9.5393920141694561</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>3</v>
       </c>
-      <c r="E2">
-        <f>G1*10</f>
+      <c r="I2">
+        <f>K1*10</f>
         <v>20</v>
       </c>
-      <c r="F2">
-        <f xml:space="preserve"> 2 *E2</f>
+      <c r="J2">
+        <f xml:space="preserve"> 2 *I2</f>
         <v>40</v>
       </c>
-      <c r="G2">
-        <f>E2*3</f>
+      <c r="K2">
+        <f>I2*3</f>
         <v>60</v>
       </c>
-      <c r="H2">
-        <f>E2*4</f>
+      <c r="L2">
+        <f>I2*4</f>
         <v>80</v>
       </c>
-      <c r="I2">
-        <f>E2 * 5</f>
+      <c r="M2">
+        <f>I2 * 5</f>
         <v>100</v>
-      </c>
-      <c r="L2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2">
-        <f>O1*10</f>
-        <v>10</v>
-      </c>
-      <c r="N2">
-        <f xml:space="preserve"> 2 *M2</f>
-        <v>20</v>
-      </c>
-      <c r="O2">
-        <f>M2*3</f>
-        <v>30</v>
-      </c>
-      <c r="P2">
-        <f>M2*4</f>
-        <v>40</v>
-      </c>
-      <c r="Q2">
-        <f>M2 * 5</f>
-        <v>50</v>
       </c>
       <c r="S2" t="s">
         <v>3</v>
@@ -4825,7 +5007,7 @@
         <v>23.25</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>174592</v>
       </c>
@@ -4836,44 +5018,24 @@
         <f t="shared" ref="C3:C12" si="0">SQRT(B3)</f>
         <v>10.099504938362077</v>
       </c>
-      <c r="E3">
-        <f>I1</f>
+      <c r="I3">
+        <f>M1</f>
         <v>0.05</v>
       </c>
-      <c r="F3">
-        <f xml:space="preserve"> 2 *E3</f>
+      <c r="J3">
+        <f xml:space="preserve"> 2 *I3</f>
         <v>0.1</v>
       </c>
-      <c r="G3">
-        <f>E3*3</f>
+      <c r="K3">
+        <f>I3*3</f>
         <v>0.15000000000000002</v>
       </c>
-      <c r="H3">
-        <f>E3*4</f>
+      <c r="L3">
+        <f>I3*4</f>
         <v>0.2</v>
       </c>
-      <c r="I3">
-        <f>E3 * 5</f>
-        <v>0.25</v>
-      </c>
       <c r="M3">
-        <f>Q1</f>
-        <v>0.05</v>
-      </c>
-      <c r="N3">
-        <f xml:space="preserve"> 2 *M3</f>
-        <v>0.1</v>
-      </c>
-      <c r="O3">
-        <f>M3*3</f>
-        <v>0.15000000000000002</v>
-      </c>
-      <c r="P3">
-        <f>M3*4</f>
-        <v>0.2</v>
-      </c>
-      <c r="Q3">
-        <f>M3 * 5</f>
+        <f>I3 * 5</f>
         <v>0.25</v>
       </c>
       <c r="S3" t="s">
@@ -4900,7 +5062,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>176497</v>
       </c>
@@ -4911,42 +5073,24 @@
         <f t="shared" si="0"/>
         <v>10.440306508910551</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H4" t="s">
         <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" t="s">
-        <v>4</v>
       </c>
       <c r="I4" t="s">
         <v>4</v>
       </c>
+      <c r="J4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" t="s">
+        <v>4</v>
+      </c>
       <c r="L4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M4" t="s">
         <v>4</v>
       </c>
-      <c r="N4" t="s">
-        <v>4</v>
-      </c>
-      <c r="O4" t="s">
-        <v>4</v>
-      </c>
-      <c r="P4" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>4</v>
-      </c>
       <c r="S4" t="s">
         <v>8</v>
       </c>
@@ -4966,7 +5110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>176656</v>
       </c>
@@ -4977,41 +5121,23 @@
         <f t="shared" si="0"/>
         <v>9.1651513899116797</v>
       </c>
-      <c r="D5">
+      <c r="H5">
         <v>1</v>
       </c>
-      <c r="E5">
+      <c r="I5">
         <v>99449</v>
       </c>
-      <c r="F5">
+      <c r="J5">
         <v>56540</v>
       </c>
-      <c r="G5">
+      <c r="K5">
         <v>31269</v>
       </c>
-      <c r="H5">
+      <c r="L5">
         <v>18510</v>
       </c>
-      <c r="I5">
+      <c r="M5">
         <v>14582</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>86060</v>
-      </c>
-      <c r="N5">
-        <v>36751</v>
-      </c>
-      <c r="O5">
-        <v>17420</v>
-      </c>
-      <c r="P5">
-        <v>10915</v>
-      </c>
-      <c r="Q5">
-        <v>5597</v>
       </c>
       <c r="S5">
         <v>1</v>
@@ -5032,7 +5158,7 @@
         <v>5473</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>175339</v>
       </c>
@@ -5043,41 +5169,23 @@
         <f t="shared" si="0"/>
         <v>10.723805294763608</v>
       </c>
-      <c r="D6">
+      <c r="H6">
         <v>2</v>
       </c>
-      <c r="E6">
+      <c r="I6">
         <v>96660</v>
       </c>
-      <c r="F6">
+      <c r="J6">
         <v>54889</v>
       </c>
-      <c r="G6">
+      <c r="K6">
         <v>31046</v>
       </c>
-      <c r="H6">
+      <c r="L6">
         <v>18576</v>
       </c>
-      <c r="I6">
+      <c r="M6">
         <v>14382</v>
-      </c>
-      <c r="L6">
-        <v>2</v>
-      </c>
-      <c r="M6">
-        <v>83472</v>
-      </c>
-      <c r="N6">
-        <v>36381</v>
-      </c>
-      <c r="O6">
-        <v>17523</v>
-      </c>
-      <c r="P6">
-        <v>10607</v>
-      </c>
-      <c r="Q6">
-        <v>5382</v>
       </c>
       <c r="S6">
         <v>2</v>
@@ -5098,7 +5206,7 @@
         <v>5675</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>174979</v>
       </c>
@@ -5109,41 +5217,23 @@
         <f t="shared" si="0"/>
         <v>10.583005244258363</v>
       </c>
-      <c r="D7">
+      <c r="H7">
         <v>3</v>
       </c>
-      <c r="E7">
+      <c r="I7">
         <v>96237</v>
       </c>
-      <c r="F7">
+      <c r="J7">
         <v>53871</v>
       </c>
-      <c r="G7">
+      <c r="K7">
         <v>31583</v>
       </c>
-      <c r="H7">
+      <c r="L7">
         <v>18396</v>
       </c>
-      <c r="I7">
+      <c r="M7">
         <v>14727</v>
-      </c>
-      <c r="L7">
-        <v>3</v>
-      </c>
-      <c r="M7">
-        <v>82578</v>
-      </c>
-      <c r="N7">
-        <v>37014</v>
-      </c>
-      <c r="O7">
-        <v>17256</v>
-      </c>
-      <c r="P7">
-        <v>10522</v>
-      </c>
-      <c r="Q7">
-        <v>5410</v>
       </c>
       <c r="S7">
         <v>3</v>
@@ -5164,7 +5254,7 @@
         <v>5608</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>174326</v>
       </c>
@@ -5175,41 +5265,23 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="D8">
+      <c r="H8">
         <v>4</v>
       </c>
-      <c r="E8">
+      <c r="I8">
         <v>95878</v>
       </c>
-      <c r="F8">
+      <c r="J8">
         <v>54345</v>
       </c>
-      <c r="G8">
+      <c r="K8">
         <v>31274</v>
       </c>
-      <c r="H8">
+      <c r="L8">
         <v>18532</v>
       </c>
-      <c r="I8">
+      <c r="M8">
         <v>14302</v>
-      </c>
-      <c r="L8">
-        <v>4</v>
-      </c>
-      <c r="M8">
-        <v>82562</v>
-      </c>
-      <c r="N8">
-        <v>36130</v>
-      </c>
-      <c r="O8">
-        <v>17471</v>
-      </c>
-      <c r="P8">
-        <v>10553</v>
-      </c>
-      <c r="Q8">
-        <v>5555</v>
       </c>
       <c r="S8">
         <v>4</v>
@@ -5230,7 +5302,7 @@
         <v>5697</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>175246</v>
       </c>
@@ -5241,68 +5313,48 @@
         <f t="shared" si="0"/>
         <v>11.313708498984761</v>
       </c>
-      <c r="E9" s="1">
-        <f>AVERAGE(E5:E8)</f>
+      <c r="I9" s="1">
+        <f>AVERAGE(I5:I8)</f>
         <v>97056</v>
       </c>
-      <c r="F9" s="1">
-        <f t="shared" ref="F9:I9" si="1">AVERAGE(F5:F8)</f>
+      <c r="J9" s="1">
+        <f t="shared" ref="J9:M9" si="1">AVERAGE(J5:J8)</f>
         <v>54911.25</v>
       </c>
-      <c r="G9" s="1">
+      <c r="K9" s="1">
         <f t="shared" si="1"/>
         <v>31293</v>
       </c>
-      <c r="H9" s="1">
+      <c r="L9" s="1">
         <f t="shared" si="1"/>
         <v>18503.5</v>
       </c>
-      <c r="I9" s="1">
+      <c r="M9" s="1">
         <f t="shared" si="1"/>
         <v>14498.25</v>
       </c>
-      <c r="M9" s="1">
-        <f t="shared" ref="M9" si="2">AVERAGE(M5:M8)</f>
-        <v>83668</v>
-      </c>
-      <c r="N9" s="1">
-        <f t="shared" ref="N9" si="3">AVERAGE(N5:N8)</f>
-        <v>36569</v>
-      </c>
-      <c r="O9" s="1">
-        <f t="shared" ref="O9" si="4">AVERAGE(O5:O8)</f>
-        <v>17417.5</v>
-      </c>
-      <c r="P9" s="1">
-        <f t="shared" ref="P9:Q9" si="5">AVERAGE(P5:P8)</f>
-        <v>10649.25</v>
-      </c>
-      <c r="Q9" s="1">
-        <f t="shared" si="5"/>
-        <v>5486</v>
-      </c>
       <c r="T9" s="1">
-        <f t="shared" ref="T9" si="6">AVERAGE(T5:T8)</f>
+        <f t="shared" ref="T9" si="2">AVERAGE(T5:T8)</f>
         <v>83394.5</v>
       </c>
       <c r="U9" s="1">
-        <f t="shared" ref="U9" si="7">AVERAGE(U5:U8)</f>
+        <f t="shared" ref="U9" si="3">AVERAGE(U5:U8)</f>
         <v>36043</v>
       </c>
       <c r="V9" s="1">
-        <f t="shared" ref="V9" si="8">AVERAGE(V5:V8)</f>
+        <f t="shared" ref="V9" si="4">AVERAGE(V5:V8)</f>
         <v>17580.5</v>
       </c>
       <c r="W9" s="1">
-        <f t="shared" ref="W9" si="9">AVERAGE(W5:W8)</f>
+        <f t="shared" ref="W9" si="5">AVERAGE(W5:W8)</f>
         <v>10792.25</v>
       </c>
       <c r="X9" s="1">
-        <f t="shared" ref="X9" si="10">AVERAGE(X5:X8)</f>
+        <f t="shared" ref="X9" si="6">AVERAGE(X5:X8)</f>
         <v>5613.25</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>175186</v>
       </c>
@@ -5313,51 +5365,28 @@
         <f t="shared" si="0"/>
         <v>11.74734012447073</v>
       </c>
-      <c r="D10" t="s">
+      <c r="H10" t="s">
         <v>12</v>
       </c>
-      <c r="E10">
-        <f>LN(E9-$B$12)</f>
+      <c r="I10">
+        <f>LN(I9-$B$12)</f>
         <v>11.481897023337551</v>
       </c>
-      <c r="F10">
-        <f t="shared" ref="F10:I10" si="11">LN(F9-$B$12)</f>
+      <c r="J10">
+        <f>LN(J9-$B$12)</f>
         <v>10.911446385344449</v>
       </c>
-      <c r="G10">
-        <f t="shared" si="11"/>
+      <c r="K10">
+        <f>LN(K9-$B$12)</f>
         <v>10.347589870259158</v>
       </c>
-      <c r="H10">
-        <f t="shared" si="11"/>
+      <c r="L10">
+        <f>LN(L9-$B$12)</f>
         <v>9.8196873777497444</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="11"/>
-        <v>9.5740837753906938</v>
-      </c>
-      <c r="L10" t="s">
-        <v>12</v>
       </c>
       <c r="M10">
         <f>LN(M9-$B$12)</f>
-        <v>11.33328191910187</v>
-      </c>
-      <c r="N10">
-        <f t="shared" ref="N10:Q10" si="12">LN(N9-$B$12)</f>
-        <v>10.503910706313379</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="12"/>
-        <v>9.7588258760447477</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="12"/>
-        <v>9.26274779549132</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="12"/>
-        <v>8.5894766430012552</v>
+        <v>9.5740837753906938</v>
       </c>
       <c r="S10" t="s">
         <v>12</v>
@@ -5367,23 +5396,23 @@
         <v>11.330003327864016</v>
       </c>
       <c r="U10">
-        <f t="shared" ref="U10:X10" si="13">LN(U9-$B$12)</f>
+        <f t="shared" ref="U10:X10" si="7">LN(U9-$B$12)</f>
         <v>10.489377976264365</v>
       </c>
       <c r="V10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>9.76820033363615</v>
       </c>
       <c r="W10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>9.2762264222883637</v>
       </c>
       <c r="X10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>8.6128760290477349</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>173851</v>
       </c>
@@ -5397,68 +5426,28 @@
       <c r="D11" t="s">
         <v>11</v>
       </c>
-      <c r="E11">
-        <f>(SQRT(E5) + SQRT(E6) + SQRT(E7) + SQRT(E8))/4</f>
-        <v>311.52997160186567</v>
-      </c>
-      <c r="F11">
-        <f t="shared" ref="F11:I11" si="14">(SQRT(F5) + SQRT(F6) + SQRT(F7) + SQRT(F8))/4</f>
-        <v>234.32170989982677</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="14"/>
-        <v>176.89745221436556</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="14"/>
-        <v>136.02735110469058</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="14"/>
-        <v>120.40668747814358</v>
-      </c>
-      <c r="M11">
-        <f>(SQRT(M5) + SQRT(M6) + SQRT(M7) + SQRT(M8))/4</f>
-        <v>289.24374519660012</v>
-      </c>
-      <c r="N11">
-        <f t="shared" ref="N11:Q11" si="15">(SQRT(N5) + SQRT(N6) + SQRT(N7) + SQRT(N8))/4</f>
-        <v>191.22817574535065</v>
-      </c>
-      <c r="O11">
-        <f t="shared" si="15"/>
-        <v>131.97483046266944</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="15"/>
-        <v>103.19244107945373</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="15"/>
-        <v>74.064947647871691</v>
-      </c>
       <c r="T11">
         <f>(SQRT(T5) + SQRT(T6) + SQRT(T7) + SQRT(T8))/4</f>
         <v>288.76644411304727</v>
       </c>
       <c r="U11">
-        <f t="shared" ref="U11:X11" si="16">(SQRT(U5) + SQRT(U6) + SQRT(U7) + SQRT(U8))/4</f>
+        <f t="shared" ref="U11:X11" si="8">(SQRT(U5) + SQRT(U6) + SQRT(U7) + SQRT(U8))/4</f>
         <v>189.84942301127268</v>
       </c>
       <c r="V11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="8"/>
         <v>132.58667410974573</v>
       </c>
       <c r="W11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="8"/>
         <v>103.88102716432491</v>
       </c>
       <c r="X11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="8"/>
         <v>74.91934436979362</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>AVERAGE(A2:A11)</f>
         <v>175354.3</v>
@@ -5468,158 +5457,1392 @@
         <v>111.2</v>
       </c>
       <c r="C12">
-        <f>AVERAGE(C2:C11)</f>
-        <v>10.519521925808958</v>
+        <f>SQRT(DEVSQ(B2:B11)/90)</f>
+        <v>5.1094683350292591</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="F14" t="s">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13" t="s">
+        <v>17</v>
+      </c>
+      <c r="M13" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" t="s">
+        <v>12</v>
+      </c>
+      <c r="O13" t="s">
+        <v>18</v>
+      </c>
+      <c r="P13" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>21</v>
+      </c>
+      <c r="R13" t="s">
+        <v>19</v>
+      </c>
+      <c r="S13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="G14" t="s">
+      <c r="C14" t="s">
         <v>6</v>
       </c>
-      <c r="H14">
+      <c r="D14">
         <v>1.99</v>
       </c>
-      <c r="I14" t="s">
+      <c r="E14" t="s">
         <v>7</v>
       </c>
-      <c r="J14">
+      <c r="F14">
         <v>0.05</v>
       </c>
+      <c r="G14">
+        <f>H14/10</f>
+        <v>2</v>
+      </c>
+      <c r="H14" s="4">
+        <v>20</v>
+      </c>
+      <c r="I14">
+        <f>I3</f>
+        <v>0.05</v>
+      </c>
+      <c r="J14" s="6">
+        <f>I9</f>
+        <v>97056</v>
+      </c>
+      <c r="K14" s="6">
+        <f>SQRT(DEVSQ(I5:I8)/12)</f>
+        <v>813.51654357281916</v>
+      </c>
+      <c r="L14" s="6">
+        <f>J14-$B$12</f>
+        <v>96944.8</v>
+      </c>
+      <c r="M14" s="6">
+        <f>SQRT(SUMSQ(K14,$C$12))</f>
+        <v>813.53258898051115</v>
+      </c>
+      <c r="N14" s="5">
+        <f>LN(L14)</f>
+        <v>11.481897023337551</v>
+      </c>
+      <c r="O14" s="5">
+        <f>M14/L14</f>
+        <v>8.3917093952487511E-3</v>
+      </c>
+      <c r="P14">
+        <f>_xlfn.COVARIANCE.P(G14:G18,N14:N18)/_xlfn.VAR.P(G14:G18)</f>
+        <v>-0.24536927517442092</v>
+      </c>
+      <c r="Q14">
+        <f>SQRT(_xlfn.VAR.P(N14:N18)/_xlfn.VAR.P(G14:G18) - P14* P14)/SQRT(5)</f>
+        <v>1.4466070771732054E-2</v>
+      </c>
+      <c r="R14" s="5">
+        <f>-P14</f>
+        <v>0.24536927517442092</v>
+      </c>
+      <c r="S14" s="5">
+        <f>Q14</f>
+        <v>1.4466070771732054E-2</v>
+      </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="F15">
-        <f>H14*10</f>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <f>D14*10</f>
         <v>19.899999999999999</v>
       </c>
+      <c r="C15">
+        <f>2*B15</f>
+        <v>39.799999999999997</v>
+      </c>
+      <c r="D15">
+        <f>B15*3</f>
+        <v>59.699999999999996</v>
+      </c>
       <c r="G15">
-        <f>2*F15</f>
+        <f t="shared" ref="G15:G18" si="9">H15/10</f>
+        <v>4</v>
+      </c>
+      <c r="H15" s="3">
+        <v>40</v>
+      </c>
+      <c r="I15">
+        <f>I14+$I$14</f>
+        <v>0.1</v>
+      </c>
+      <c r="J15" s="6">
+        <f>J9</f>
+        <v>54911.25</v>
+      </c>
+      <c r="K15" s="6">
+        <f>SQRT(DEVSQ(J5:J8)/12)</f>
+        <v>581.38346138041004</v>
+      </c>
+      <c r="L15" s="6">
+        <f t="shared" ref="L15:L18" si="10">J15-$B$12</f>
+        <v>54800.05</v>
+      </c>
+      <c r="M15" s="6">
+        <f t="shared" ref="M15:M18" si="11">SQRT(SUMSQ(K15,$C$12))</f>
+        <v>581.40591313929156</v>
+      </c>
+      <c r="N15" s="5">
+        <f t="shared" ref="N15:N18" si="12">LN(L15)</f>
+        <v>10.911446385344449</v>
+      </c>
+      <c r="O15" s="5">
+        <f t="shared" ref="O15:O18" si="13">M15/L15</f>
+        <v>1.0609587274816201E-2</v>
+      </c>
+      <c r="V15" t="s">
+        <v>5</v>
+      </c>
+      <c r="W15" t="s">
+        <v>6</v>
+      </c>
+      <c r="X15">
+        <v>1</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z15">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="H16" s="4">
+        <v>60</v>
+      </c>
+      <c r="I16">
+        <f t="shared" ref="I16:I18" si="14">I15+$I$14</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="J16" s="6">
+        <f>K9</f>
+        <v>31293</v>
+      </c>
+      <c r="K16" s="6">
+        <f>SQRT(DEVSQ(K5:K8)/12)</f>
+        <v>110.31998912255204</v>
+      </c>
+      <c r="L16" s="6">
+        <f t="shared" si="10"/>
+        <v>31181.8</v>
+      </c>
+      <c r="M16" s="6">
+        <f t="shared" si="11"/>
+        <v>110.4382482053508</v>
+      </c>
+      <c r="N16" s="5">
+        <f t="shared" si="12"/>
+        <v>10.347589870259158</v>
+      </c>
+      <c r="O16" s="5">
+        <f t="shared" si="13"/>
+        <v>3.5417534653339705E-3</v>
+      </c>
+      <c r="P16" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q16">
+        <v>2.7</v>
+      </c>
+      <c r="R16" t="s">
+        <v>18</v>
+      </c>
+      <c r="S16">
+        <v>0.1</v>
+      </c>
+      <c r="U16" t="s">
+        <v>3</v>
+      </c>
+      <c r="V16">
+        <f>X15*10</f>
+        <v>10</v>
+      </c>
+      <c r="W16">
+        <f xml:space="preserve"> 2 *V16</f>
+        <v>20</v>
+      </c>
+      <c r="X16">
+        <f>V16*3</f>
+        <v>30</v>
+      </c>
+      <c r="Y16">
+        <f>V16*4</f>
+        <v>40</v>
+      </c>
+      <c r="Z16">
+        <f>V16 * 5</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>180252</v>
+      </c>
+      <c r="C17">
+        <v>168047</v>
+      </c>
+      <c r="D17">
+        <v>161133</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="H17" s="3">
+        <v>80</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="14"/>
+        <v>0.2</v>
+      </c>
+      <c r="J17" s="6">
+        <f>L9</f>
+        <v>18503.5</v>
+      </c>
+      <c r="K17" s="6">
+        <f>SQRT(DEVSQ(L5:L8)/12)</f>
+        <v>38.369910085899342</v>
+      </c>
+      <c r="L17" s="6">
+        <f t="shared" si="10"/>
+        <v>18392.3</v>
+      </c>
+      <c r="M17" s="6">
+        <f t="shared" si="11"/>
+        <v>38.708612306135009</v>
+      </c>
+      <c r="N17" s="5">
+        <f t="shared" si="12"/>
+        <v>9.8196873777497444</v>
+      </c>
+      <c r="O17" s="5">
+        <f t="shared" si="13"/>
+        <v>2.1046096630728626E-3</v>
+      </c>
+      <c r="V17">
+        <f>Z15</f>
+        <v>0.1</v>
+      </c>
+      <c r="W17">
+        <f xml:space="preserve"> 2 *V17</f>
+        <v>0.2</v>
+      </c>
+      <c r="X17">
+        <f>V17*3</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="Y17">
+        <f>V17*4</f>
+        <v>0.4</v>
+      </c>
+      <c r="Z17">
+        <f>V17 * 5</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>180248</v>
+      </c>
+      <c r="C18">
+        <v>168313</v>
+      </c>
+      <c r="D18">
+        <v>161073</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="H18" s="3">
+        <v>100</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" si="14"/>
+        <v>0.25</v>
+      </c>
+      <c r="J18" s="6">
+        <f>M9</f>
+        <v>14498.25</v>
+      </c>
+      <c r="K18" s="6">
+        <f>SQRT(DEVSQ(M5:M8)/12)</f>
+        <v>96.336541180730933</v>
+      </c>
+      <c r="L18" s="6">
+        <f t="shared" si="10"/>
+        <v>14387.05</v>
+      </c>
+      <c r="M18" s="6">
+        <f t="shared" si="11"/>
+        <v>96.471943244309813</v>
+      </c>
+      <c r="N18" s="5">
+        <f t="shared" si="12"/>
+        <v>9.5740837753906938</v>
+      </c>
+      <c r="O18" s="5">
+        <f t="shared" si="13"/>
+        <v>6.7054707701933213E-3</v>
+      </c>
+      <c r="P18" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q18" s="5">
+        <f>R14/Q16</f>
+        <v>9.0877509323859587E-2</v>
+      </c>
+      <c r="R18" t="s">
+        <v>18</v>
+      </c>
+      <c r="S18" s="5">
+        <f>SQRT(SUMSQ(S14/Q16,R14*S16/Q16^2))</f>
+        <v>6.3273138014989854E-3</v>
+      </c>
+      <c r="U18" t="s">
+        <v>8</v>
+      </c>
+      <c r="V18" t="s">
+        <v>4</v>
+      </c>
+      <c r="W18" t="s">
+        <v>4</v>
+      </c>
+      <c r="X18" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>177296</v>
+      </c>
+      <c r="C19">
+        <v>166665</v>
+      </c>
+      <c r="D19">
+        <v>160431</v>
+      </c>
+      <c r="U19">
+        <v>1</v>
+      </c>
+      <c r="V19">
+        <v>86060</v>
+      </c>
+      <c r="W19">
+        <v>36751</v>
+      </c>
+      <c r="X19">
+        <v>17420</v>
+      </c>
+      <c r="Y19">
+        <v>10915</v>
+      </c>
+      <c r="Z19">
+        <v>5597</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>175960</v>
+      </c>
+      <c r="C20">
+        <v>166630</v>
+      </c>
+      <c r="D20">
+        <v>161017</v>
+      </c>
+      <c r="U20">
+        <v>2</v>
+      </c>
+      <c r="V20">
+        <v>83472</v>
+      </c>
+      <c r="W20">
+        <v>36381</v>
+      </c>
+      <c r="X20">
+        <v>17523</v>
+      </c>
+      <c r="Y20">
+        <v>10607</v>
+      </c>
+      <c r="Z20">
+        <v>5382</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B21" s="1">
+        <f t="shared" ref="B21" si="15">AVERAGE(B17:B20)</f>
+        <v>178439</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" ref="C21" si="16">AVERAGE(C17:C20)</f>
+        <v>167413.75</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" ref="D21" si="17">AVERAGE(D17:D20)</f>
+        <v>160913.5</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="H21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" t="s">
+        <v>16</v>
+      </c>
+      <c r="L21" t="s">
+        <v>17</v>
+      </c>
+      <c r="M21" t="s">
+        <v>18</v>
+      </c>
+      <c r="N21" t="s">
+        <v>12</v>
+      </c>
+      <c r="O21" t="s">
+        <v>18</v>
+      </c>
+      <c r="P21" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>21</v>
+      </c>
+      <c r="R21" t="s">
+        <v>19</v>
+      </c>
+      <c r="S21" t="s">
+        <v>22</v>
+      </c>
+      <c r="U21">
+        <v>3</v>
+      </c>
+      <c r="V21">
+        <v>82578</v>
+      </c>
+      <c r="W21">
+        <v>37014</v>
+      </c>
+      <c r="X21">
+        <v>17256</v>
+      </c>
+      <c r="Y21">
+        <v>10522</v>
+      </c>
+      <c r="Z21">
+        <v>5410</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <f>LN(B21-$B$12)</f>
+        <v>12.091378708691272</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ref="C22:D22" si="18">LN(C21-$B$12)</f>
+        <v>12.027559128938851</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="18"/>
+        <v>11.987930939107295</v>
+      </c>
+      <c r="G22">
+        <f>H22/10</f>
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="H22" s="4">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="I22">
+        <f>X1</f>
+        <v>0.05</v>
+      </c>
+      <c r="J22" s="6">
+        <f>T9</f>
+        <v>83394.5</v>
+      </c>
+      <c r="K22" s="6">
+        <f>SQRT(DEVSQ(T5:T8)/12)</f>
+        <v>971.87357716937652</v>
+      </c>
+      <c r="L22" s="6">
+        <f>J22-$B$12</f>
+        <v>83283.3</v>
+      </c>
+      <c r="M22" s="6">
+        <f>SQRT(SUMSQ(K22,$C$12))</f>
+        <v>971.88700817876293</v>
+      </c>
+      <c r="N22" s="5">
+        <f>LN(L22)</f>
+        <v>11.330003327864016</v>
+      </c>
+      <c r="O22" s="5">
+        <f>M22/L22</f>
+        <v>1.1669650556339181E-2</v>
+      </c>
+      <c r="P22">
+        <f>_xlfn.COVARIANCE.P(G22:G26,N22:N26)/_xlfn.VAR.P(G22:G26)</f>
+        <v>-1.429549710023347</v>
+      </c>
+      <c r="Q22">
+        <f>SQRT(_xlfn.VAR.P(N22:N26)/_xlfn.VAR.P(G22:G26) - P22* P22)/SQRT(5)</f>
+        <v>5.8119512567118614E-2</v>
+      </c>
+      <c r="R22">
+        <f>-P22</f>
+        <v>1.429549710023347</v>
+      </c>
+      <c r="S22">
+        <f>Q22</f>
+        <v>5.8119512567118614E-2</v>
+      </c>
+      <c r="U22">
+        <v>4</v>
+      </c>
+      <c r="V22">
+        <v>82562</v>
+      </c>
+      <c r="W22">
+        <v>36130</v>
+      </c>
+      <c r="X22">
+        <v>17471</v>
+      </c>
+      <c r="Y22">
+        <v>10553</v>
+      </c>
+      <c r="Z22">
+        <v>5555</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <f>(SQRT(B17) + SQRT(B18) + SQRT(B19) + SQRT(B20))/4</f>
+        <v>422.41459190727431</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23:D23" si="19">(SQRT(C17) + SQRT(C18) + SQRT(C19) + SQRT(C20))/4</f>
+        <v>409.16116613063099</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="19"/>
+        <v>401.14009610613527</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ref="G23:G26" si="20">H23/10</f>
+        <v>0.93</v>
+      </c>
+      <c r="H23" s="3">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="I23">
+        <f>I22+$I$14</f>
+        <v>0.1</v>
+      </c>
+      <c r="J23" s="6">
+        <f>U9</f>
+        <v>36043</v>
+      </c>
+      <c r="K23" s="6">
+        <f>SQRT(DEVSQ(U5:U8)/12)</f>
+        <v>97.28651842196156</v>
+      </c>
+      <c r="L23" s="6">
+        <f t="shared" ref="L23:L26" si="21">J23-$B$12</f>
+        <v>35931.800000000003</v>
+      </c>
+      <c r="M23" s="6">
+        <f t="shared" ref="M23:M26" si="22">SQRT(SUMSQ(K23,$C$12))</f>
+        <v>97.420600148702292</v>
+      </c>
+      <c r="N23" s="5">
+        <f t="shared" ref="N23:N26" si="23">LN(L23)</f>
+        <v>10.489377976264365</v>
+      </c>
+      <c r="O23" s="5">
+        <f t="shared" ref="O23:O26" si="24">M23/L23</f>
+        <v>2.7112641211601502E-3</v>
+      </c>
+      <c r="V23" s="1">
+        <f t="shared" ref="V23" si="25">AVERAGE(V19:V22)</f>
+        <v>83668</v>
+      </c>
+      <c r="W23" s="1">
+        <f t="shared" ref="W23" si="26">AVERAGE(W19:W22)</f>
+        <v>36569</v>
+      </c>
+      <c r="X23" s="1">
+        <f t="shared" ref="X23" si="27">AVERAGE(X19:X22)</f>
+        <v>17417.5</v>
+      </c>
+      <c r="Y23" s="1">
+        <f t="shared" ref="Y23:Z23" si="28">AVERAGE(Y19:Y22)</f>
+        <v>10649.25</v>
+      </c>
+      <c r="Z23" s="1">
+        <f t="shared" si="28"/>
+        <v>5486</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <f t="shared" si="20"/>
+        <v>1.395</v>
+      </c>
+      <c r="H24" s="4">
+        <v>13.95</v>
+      </c>
+      <c r="I24">
+        <f t="shared" ref="I24:I26" si="29">I23+$I$14</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="J24" s="6">
+        <f>V9</f>
+        <v>17580.5</v>
+      </c>
+      <c r="K24" s="6">
+        <f>SQRT(DEVSQ(V5:V8)/12)</f>
+        <v>173.01950757067829</v>
+      </c>
+      <c r="L24" s="6">
+        <f t="shared" si="21"/>
+        <v>17469.3</v>
+      </c>
+      <c r="M24" s="6">
+        <f t="shared" si="22"/>
+        <v>173.09493541599264</v>
+      </c>
+      <c r="N24" s="5">
+        <f t="shared" si="23"/>
+        <v>9.76820033363615</v>
+      </c>
+      <c r="O24" s="5">
+        <f t="shared" si="24"/>
+        <v>9.9085215444232252E-3</v>
+      </c>
+      <c r="P24" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q24">
+        <v>11.337</v>
+      </c>
+      <c r="R24" t="s">
+        <v>18</v>
+      </c>
+      <c r="S24">
+        <v>1E-3</v>
+      </c>
+      <c r="U24" t="s">
+        <v>12</v>
+      </c>
+      <c r="V24">
+        <f>LN(V23-$B$12)</f>
+        <v>11.33328191910187</v>
+      </c>
+      <c r="W24">
+        <f t="shared" ref="W24:Z24" si="30">LN(W23-$B$12)</f>
+        <v>10.503910706313379</v>
+      </c>
+      <c r="X24">
+        <f t="shared" si="30"/>
+        <v>9.7588258760447477</v>
+      </c>
+      <c r="Y24">
+        <f t="shared" si="30"/>
+        <v>9.26274779549132</v>
+      </c>
+      <c r="Z24">
+        <f t="shared" si="30"/>
+        <v>8.5894766430012552</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <f t="shared" si="20"/>
+        <v>1.86</v>
+      </c>
+      <c r="H25" s="3">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="29"/>
+        <v>0.2</v>
+      </c>
+      <c r="J25" s="6">
+        <f>W9</f>
+        <v>10792.25</v>
+      </c>
+      <c r="K25" s="6">
+        <f>SQRT(DEVSQ(W5:W8)/12)</f>
+        <v>118.64047580821648</v>
+      </c>
+      <c r="L25" s="6">
+        <f t="shared" si="21"/>
+        <v>10681.05</v>
+      </c>
+      <c r="M25" s="6">
+        <f t="shared" si="22"/>
+        <v>118.75044912195771</v>
+      </c>
+      <c r="N25" s="5">
+        <f t="shared" si="23"/>
+        <v>9.2762264222883637</v>
+      </c>
+      <c r="O25" s="5">
+        <f t="shared" si="24"/>
+        <v>1.1117862861980585E-2</v>
+      </c>
+      <c r="V25">
+        <f>(SQRT(V19) + SQRT(V20) + SQRT(V21) + SQRT(V22))/4</f>
+        <v>289.24374519660012</v>
+      </c>
+      <c r="W25">
+        <f t="shared" ref="W25:Z25" si="31">(SQRT(W19) + SQRT(W20) + SQRT(W21) + SQRT(W22))/4</f>
+        <v>191.22817574535065</v>
+      </c>
+      <c r="X25">
+        <f t="shared" si="31"/>
+        <v>131.97483046266944</v>
+      </c>
+      <c r="Y25">
+        <f t="shared" si="31"/>
+        <v>103.19244107945373</v>
+      </c>
+      <c r="Z25">
+        <f t="shared" si="31"/>
+        <v>74.064947647871691</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="G26">
+        <f t="shared" si="20"/>
+        <v>2.3250000000000002</v>
+      </c>
+      <c r="H26" s="3">
+        <v>23.25</v>
+      </c>
+      <c r="I26" s="3">
+        <f t="shared" si="29"/>
+        <v>0.25</v>
+      </c>
+      <c r="J26" s="6">
+        <f>X9</f>
+        <v>5613.25</v>
+      </c>
+      <c r="K26" s="6">
+        <f>SQRT(DEVSQ(X5:X8)/12)</f>
+        <v>50.435395970158361</v>
+      </c>
+      <c r="L26" s="6">
+        <f t="shared" si="21"/>
+        <v>5502.05</v>
+      </c>
+      <c r="M26" s="6">
+        <f t="shared" si="22"/>
+        <v>50.693548241697705</v>
+      </c>
+      <c r="N26" s="5">
+        <f t="shared" si="23"/>
+        <v>8.6128760290477349</v>
+      </c>
+      <c r="O26" s="5">
+        <f t="shared" si="24"/>
+        <v>9.2135746206773294E-3</v>
+      </c>
+      <c r="P26" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q26" s="5">
+        <f>R22/Q24</f>
+        <v>0.12609594337332161</v>
+      </c>
+      <c r="R26" t="s">
+        <v>18</v>
+      </c>
+      <c r="S26" s="5">
+        <f>SQRT(SUMSQ(S22/Q24,R22*S24/Q24^2))</f>
+        <v>5.1265457665760879E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>0.4</v>
+      </c>
+      <c r="B29">
+        <v>0.6</v>
+      </c>
+      <c r="C29">
+        <v>0.5</v>
+      </c>
+      <c r="D29">
+        <v>0.5</v>
+      </c>
+      <c r="H29" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" t="s">
+        <v>15</v>
+      </c>
+      <c r="K29" t="s">
+        <v>16</v>
+      </c>
+      <c r="L29" t="s">
+        <v>17</v>
+      </c>
+      <c r="M29" t="s">
+        <v>18</v>
+      </c>
+      <c r="N29" t="s">
+        <v>12</v>
+      </c>
+      <c r="O29" t="s">
+        <v>18</v>
+      </c>
+      <c r="P29" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>21</v>
+      </c>
+      <c r="R29" t="s">
+        <v>19</v>
+      </c>
+      <c r="S29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="G30">
+        <f>H30/10</f>
+        <v>1</v>
+      </c>
+      <c r="H30" s="3">
+        <v>10</v>
+      </c>
+      <c r="I30">
+        <f>Z15</f>
+        <v>0.1</v>
+      </c>
+      <c r="J30" s="6">
+        <f>V23</f>
+        <v>83668</v>
+      </c>
+      <c r="K30" s="6">
+        <f>SQRT(DEVSQ(V19:V22)/12)</f>
+        <v>825.19775407676275</v>
+      </c>
+      <c r="L30" s="6">
+        <f>J30-$B$12</f>
+        <v>83556.800000000003</v>
+      </c>
+      <c r="M30" s="6">
+        <f>SQRT(SUMSQ(K30,$C$12))</f>
+        <v>825.21357235566609</v>
+      </c>
+      <c r="N30" s="5">
+        <f>LN(L30)</f>
+        <v>11.33328191910187</v>
+      </c>
+      <c r="O30" s="5">
+        <f>M30/L30</f>
+        <v>9.8760791743540445E-3</v>
+      </c>
+      <c r="P30">
+        <f>_xlfn.COVARIANCE.P(G30:G34,N30:N34)/_xlfn.VAR.P(G30:G34)</f>
+        <v>-0.67287734630232876</v>
+      </c>
+      <c r="Q30">
+        <f>SQRT(_xlfn.VAR.P(N30:N34)/_xlfn.VAR.P(G30:G34) - P30* P30)/SQRT(5)</f>
+        <v>2.6200070674574763E-2</v>
+      </c>
+      <c r="R30">
+        <f>-P30</f>
+        <v>0.67287734630232876</v>
+      </c>
+      <c r="S30">
+        <f>Q30</f>
+        <v>2.6200070674574763E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="G31">
+        <f t="shared" ref="G31:G34" si="32">H31/10</f>
+        <v>2</v>
+      </c>
+      <c r="H31" s="3">
+        <v>20</v>
+      </c>
+      <c r="I31">
+        <f>I30+$Z$15</f>
+        <v>0.2</v>
+      </c>
+      <c r="J31" s="6">
+        <f>W23</f>
+        <v>36569</v>
+      </c>
+      <c r="K31" s="6">
+        <f>SQRT(DEVSQ(W19:W22)/12)</f>
+        <v>195.62165865091046</v>
+      </c>
+      <c r="L31" s="6">
+        <f t="shared" ref="L31:L34" si="33">J31-$B$12</f>
+        <v>36457.800000000003</v>
+      </c>
+      <c r="M31" s="6">
+        <f t="shared" ref="M31:M34" si="34">SQRT(SUMSQ(K31,$C$12))</f>
+        <v>195.68837471858157</v>
+      </c>
+      <c r="N31" s="5">
+        <f t="shared" ref="N31:N34" si="35">LN(L31)</f>
+        <v>10.503910706313379</v>
+      </c>
+      <c r="O31" s="5">
+        <f t="shared" ref="O31:O34" si="36">M31/L31</f>
+        <v>5.367531083021509E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="G32">
+        <f t="shared" si="32"/>
+        <v>3</v>
+      </c>
+      <c r="H32" s="3">
+        <v>30</v>
+      </c>
+      <c r="I32">
+        <f t="shared" ref="I32:I34" si="37">I31+$Z$15</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="J32" s="6">
+        <f>X23</f>
+        <v>17417.5</v>
+      </c>
+      <c r="K32" s="6">
+        <f>SQRT(DEVSQ(X19:X22)/12)</f>
+        <v>57.793454069931947</v>
+      </c>
+      <c r="L32" s="6">
+        <f t="shared" si="33"/>
+        <v>17306.3</v>
+      </c>
+      <c r="M32" s="6">
+        <f t="shared" si="34"/>
+        <v>58.018876238686317</v>
+      </c>
+      <c r="N32" s="5">
+        <f t="shared" si="35"/>
+        <v>9.7588258760447477</v>
+      </c>
+      <c r="O32" s="5">
+        <f t="shared" si="36"/>
+        <v>3.3524714259365851E-3</v>
+      </c>
+      <c r="P32" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q32">
+        <v>7.85</v>
+      </c>
+      <c r="R32" t="s">
+        <v>18</v>
+      </c>
+      <c r="S32">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="33" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="G33">
+        <f t="shared" si="32"/>
+        <v>4</v>
+      </c>
+      <c r="H33" s="3">
+        <v>40</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="37"/>
+        <v>0.4</v>
+      </c>
+      <c r="J33" s="6">
+        <f>Y23</f>
+        <v>10649.25</v>
+      </c>
+      <c r="K33" s="6">
+        <f>SQRT(DEVSQ(Y19:Y22)/12)</f>
+        <v>90.307230238410767</v>
+      </c>
+      <c r="L33" s="6">
+        <f t="shared" si="33"/>
+        <v>10538.05</v>
+      </c>
+      <c r="M33" s="6">
+        <f t="shared" si="34"/>
+        <v>90.451658359590056</v>
+      </c>
+      <c r="N33" s="5">
+        <f t="shared" si="35"/>
+        <v>9.26274779549132</v>
+      </c>
+      <c r="O33" s="5">
+        <f t="shared" si="36"/>
+        <v>8.583339266713487E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="G34">
+        <f t="shared" si="32"/>
+        <v>5</v>
+      </c>
+      <c r="H34" s="3">
+        <v>50</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="37"/>
+        <v>0.5</v>
+      </c>
+      <c r="J34" s="6">
+        <f>Z23</f>
+        <v>5486</v>
+      </c>
+      <c r="K34" s="6">
+        <f>SQRT(DEVSQ(Z19:Z22)/12)</f>
+        <v>52.973263696573071</v>
+      </c>
+      <c r="L34" s="6">
+        <f t="shared" si="33"/>
+        <v>5374.8</v>
+      </c>
+      <c r="M34" s="6">
+        <f t="shared" si="34"/>
+        <v>53.219106844566014</v>
+      </c>
+      <c r="N34" s="5">
+        <f t="shared" si="35"/>
+        <v>8.5894766430012552</v>
+      </c>
+      <c r="O34" s="5">
+        <f t="shared" si="36"/>
+        <v>9.9015976119234232E-3</v>
+      </c>
+      <c r="P34" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q34" s="5">
+        <f>R30/Q32</f>
+        <v>8.5716859401570547E-2</v>
+      </c>
+      <c r="R34" t="s">
+        <v>18</v>
+      </c>
+      <c r="S34" s="5">
+        <f>SQRT(SUMSQ(S30/Q32,R30*S32/Q32^2))</f>
+        <v>3.3393743444899838E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="H37" t="s">
+        <v>13</v>
+      </c>
+      <c r="I37" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" t="s">
+        <v>15</v>
+      </c>
+      <c r="K37" t="s">
+        <v>16</v>
+      </c>
+      <c r="L37" t="s">
+        <v>17</v>
+      </c>
+      <c r="M37" t="s">
+        <v>18</v>
+      </c>
+      <c r="N37" t="s">
+        <v>12</v>
+      </c>
+      <c r="O37" t="s">
+        <v>18</v>
+      </c>
+      <c r="P37" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>21</v>
+      </c>
+      <c r="R37" t="s">
+        <v>19</v>
+      </c>
+      <c r="S37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="G38">
+        <f>H38/10</f>
+        <v>1.9899999999999998</v>
+      </c>
+      <c r="H38" s="4">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="I38">
+        <f>F14</f>
+        <v>0.05</v>
+      </c>
+      <c r="J38" s="6">
+        <f>B21</f>
+        <v>178439</v>
+      </c>
+      <c r="K38" s="6">
+        <f>SQRT(DEVSQ(B17:B20)/12)</f>
+        <v>1080.5608111840197</v>
+      </c>
+      <c r="L38" s="6">
+        <f>J38-$B$12</f>
+        <v>178327.8</v>
+      </c>
+      <c r="M38" s="6">
+        <f>SQRT(SUMSQ(K38,$C$12))</f>
+        <v>1080.5728912633951</v>
+      </c>
+      <c r="N38" s="5">
+        <f>LN(L38)</f>
+        <v>12.091378708691272</v>
+      </c>
+      <c r="O38" s="5">
+        <f>M38/L38</f>
+        <v>6.0594752543540334E-3</v>
+      </c>
+      <c r="P38">
+        <f>_xlfn.COVARIANCE.P(G38:G42,N38:N42)/_xlfn.VAR.P(G38:G42)</f>
+        <v>-2.599190190552161E-2</v>
+      </c>
+      <c r="Q38">
+        <f>SQRT(_xlfn.VAR.P(N38:N42)/_xlfn.VAR.P(G38:G42) - P38* P38)/SQRT(5)</f>
+        <v>1.5693944771377744E-3</v>
+      </c>
+      <c r="R38">
+        <f>-P38</f>
+        <v>2.599190190552161E-2</v>
+      </c>
+      <c r="S38">
+        <f>Q38</f>
+        <v>1.5693944771377744E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="G39">
+        <f t="shared" ref="G39:G42" si="38">H39/10</f>
+        <v>3.9799999999999995</v>
+      </c>
+      <c r="H39" s="3">
         <v>39.799999999999997</v>
       </c>
-      <c r="H15">
-        <f>F15*3</f>
-        <v>59.699999999999996</v>
+      <c r="I39">
+        <f>I38+$I$14</f>
+        <v>0.1</v>
+      </c>
+      <c r="J39" s="6">
+        <f>C21</f>
+        <v>167413.75</v>
+      </c>
+      <c r="K39" s="6">
+        <f>SQRT(DEVSQ(C17:C20)/12)</f>
+        <v>445.77149882722051</v>
+      </c>
+      <c r="L39" s="6">
+        <f t="shared" ref="L39:L42" si="39">J39-$B$12</f>
+        <v>167302.54999999999</v>
+      </c>
+      <c r="M39" s="6">
+        <f t="shared" ref="M39:M42" si="40">SQRT(SUMSQ(K39,$C$12))</f>
+        <v>445.80078043149871</v>
+      </c>
+      <c r="N39" s="5">
+        <f t="shared" ref="N39:N42" si="41">LN(L39)</f>
+        <v>12.027559128938851</v>
+      </c>
+      <c r="O39" s="5">
+        <f t="shared" ref="O39:O42" si="42">M39/L39</f>
+        <v>2.6646382881282964E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="E16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" t="s">
-        <v>4</v>
-      </c>
-      <c r="G16" t="s">
-        <v>4</v>
-      </c>
-      <c r="H16" t="s">
-        <v>4</v>
+    <row r="40" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="G40">
+        <f t="shared" si="38"/>
+        <v>5.9700000000000006</v>
+      </c>
+      <c r="H40" s="4">
+        <v>59.7</v>
+      </c>
+      <c r="I40">
+        <f t="shared" ref="I40:I42" si="43">I39+$I$14</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="J40" s="6">
+        <f>D21</f>
+        <v>160913.5</v>
+      </c>
+      <c r="K40" s="6">
+        <f>SQRT(DEVSQ(D17:D20)/12)</f>
+        <v>162.56767821433633</v>
+      </c>
+      <c r="L40" s="6">
+        <f t="shared" si="39"/>
+        <v>160802.29999999999</v>
+      </c>
+      <c r="M40" s="6">
+        <f t="shared" si="40"/>
+        <v>162.64795315855244</v>
+      </c>
+      <c r="N40" s="5">
+        <f t="shared" si="41"/>
+        <v>11.987930939107295</v>
+      </c>
+      <c r="O40" s="5">
+        <f t="shared" si="42"/>
+        <v>1.0114777783561085E-3</v>
+      </c>
+      <c r="P40" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q40">
+        <v>0.24</v>
+      </c>
+      <c r="R40" t="s">
+        <v>18</v>
+      </c>
+      <c r="S40">
+        <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>180252</v>
-      </c>
-      <c r="G17">
-        <v>168047</v>
-      </c>
-      <c r="H17">
-        <v>161133</v>
-      </c>
+    <row r="41" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="H41" s="3"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
     </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E18">
-        <v>2</v>
-      </c>
-      <c r="F18">
-        <v>180248</v>
-      </c>
-      <c r="G18">
-        <v>168313</v>
-      </c>
-      <c r="H18">
-        <v>161073</v>
-      </c>
-    </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E19">
-        <v>3</v>
-      </c>
-      <c r="F19">
-        <v>177296</v>
-      </c>
-      <c r="G19">
-        <v>166665</v>
-      </c>
-      <c r="H19">
-        <v>160431</v>
-      </c>
-    </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E20">
-        <v>4</v>
-      </c>
-      <c r="F20">
-        <v>175960</v>
-      </c>
-      <c r="G20">
-        <v>166630</v>
-      </c>
-      <c r="H20">
-        <v>161017</v>
-      </c>
-    </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="F21" s="1">
-        <f t="shared" ref="F21" si="17">AVERAGE(F17:F20)</f>
-        <v>178439</v>
-      </c>
-      <c r="G21" s="1">
-        <f t="shared" ref="G21" si="18">AVERAGE(G17:G20)</f>
-        <v>167413.75</v>
-      </c>
-      <c r="H21" s="1">
-        <f t="shared" ref="H21" si="19">AVERAGE(H17:H20)</f>
-        <v>160913.5</v>
-      </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="F22">
-        <f>LN(F21-$B$12)</f>
-        <v>12.091378708691272</v>
-      </c>
-      <c r="G22">
-        <f t="shared" ref="G22:H22" si="20">LN(G21-$B$12)</f>
-        <v>12.027559128938851</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="20"/>
-        <v>11.987930939107295</v>
-      </c>
-    </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="F23">
-        <f>(SQRT(F17) + SQRT(F18) + SQRT(F19) + SQRT(F20))/4</f>
-        <v>422.41459190727431</v>
-      </c>
-      <c r="G23">
-        <f t="shared" ref="G23:H23" si="21">(SQRT(G17) + SQRT(G18) + SQRT(G19) + SQRT(G20))/4</f>
-        <v>409.16116613063099</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="21"/>
-        <v>401.14009610613527</v>
+    <row r="42" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
+      <c r="P42" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q42" s="5">
+        <f>R38/Q40</f>
+        <v>0.10829959127300672</v>
+      </c>
+      <c r="R42" t="s">
+        <v>18</v>
+      </c>
+      <c r="S42" s="5">
+        <f>SQRT(SUMSQ(S38/Q40,R38*S40/Q40^2))</f>
+        <v>4.5596169301031879E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F5FD115-8094-459C-B25E-773788E8BC30}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>